<commit_message>
first cut commit of merge
</commit_message>
<xml_diff>
--- a/app-conf/data/datarep/species/templates/genericspeciespages_mapping.xlsx
+++ b/app-conf/data/datarep/species/templates/genericspeciespages_mapping.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="164">
   <si>
     <t>S.No.</t>
   </si>
@@ -233,9 +233,6 @@
     <t>Additional taxonomic heirarchies, including contributor provided heirarchies.</t>
   </si>
   <si>
-    <t>Author Contributed Taxonomic Hierarchy</t>
-  </si>
-  <si>
     <t>Sub-Family</t>
   </si>
   <si>
@@ -398,9 +395,6 @@
     <t>Country or countries where the taxon is found. List of countries according to the ISO 3166 standard.</t>
   </si>
   <si>
-    <t>Indian Distribution Geographic Entity</t>
-  </si>
-  <si>
     <t>State or States, District or Districts, Taluk or Taluks, Biogeographic region or regions in India according to IBP standard.</t>
   </si>
   <si>
@@ -416,9 +410,6 @@
     <t>Country or countries the taxon is endemic to. List of countries according to the ISO 3166 standard.</t>
   </si>
   <si>
-    <t>Indian Endemicity Geographic Entity</t>
-  </si>
-  <si>
     <t>State or States and Biogeographic region or regions in India, according to IBP standard, that the taxon is endemic to.</t>
   </si>
   <si>
@@ -522,24 +513,35 @@
   </si>
   <si>
     <t>Links to all documents on IBP referred to/associated with/ used in this entire page</t>
+  </si>
+  <si>
+    <t>Images</t>
+  </si>
+  <si>
+    <t>Local Distribution Geographic Entity</t>
+  </si>
+  <si>
+    <t>Local Endemicity Geographic Entity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b/>
@@ -547,11 +549,13 @@
       <color rgb="FF000000"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b/>
@@ -559,6 +563,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i/>
@@ -566,23 +571,27 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Monospace"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Monospace"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -647,7 +656,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -716,11 +725,6 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -799,7 +803,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -834,7 +837,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1010,11 +1012,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P83"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:P84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E82" sqref="E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1023,7 +1025,7 @@
     <col min="2" max="2" width="14.42578125" style="1"/>
     <col min="3" max="3" width="9.7109375" style="1"/>
     <col min="4" max="4" width="14.140625" style="1"/>
-    <col min="5" max="5" width="37.28515625" style="1"/>
+    <col min="5" max="5" width="37.42578125" style="1"/>
     <col min="6" max="6" width="8.5703125"/>
     <col min="7" max="7" width="14.140625"/>
     <col min="8" max="1025" width="8.5703125"/>
@@ -1527,7 +1529,7 @@
         <v>35</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>59</v>
@@ -1598,7 +1600,7 @@
         <v>65</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>66</v>
@@ -1632,7 +1634,7 @@
         <v>65</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>66</v>
@@ -1663,10 +1665,10 @@
         <v>35</v>
       </c>
       <c r="C37" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="114.75">
@@ -1674,13 +1676,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="89.25">
@@ -1688,13 +1690,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="38.25">
@@ -1702,13 +1704,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C40" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="38.25">
@@ -1716,13 +1718,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="38.25">
@@ -1730,13 +1732,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C42" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="25.5">
@@ -1744,13 +1746,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C43" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="25.5">
@@ -1758,13 +1760,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C44" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="38.25">
@@ -1772,13 +1774,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C45" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="102">
@@ -1786,13 +1788,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C46" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="F46" s="12"/>
     </row>
@@ -1801,13 +1803,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C47" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="38.25">
@@ -1815,13 +1817,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C48" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="76.5">
@@ -1829,13 +1831,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C49" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="89.25">
@@ -1843,13 +1845,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C50" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E50" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="102">
@@ -1857,13 +1859,13 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C51" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E51" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="89.25">
@@ -1871,13 +1873,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C52" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="63.75">
@@ -1885,13 +1887,13 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C53" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1899,13 +1901,13 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C54" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="38.25">
@@ -1913,13 +1915,13 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C55" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E55" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="38.25">
@@ -1927,13 +1929,13 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C56" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E56" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="38.25">
@@ -1941,13 +1943,13 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C57" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E57" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="25.5">
@@ -1955,13 +1957,13 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C58" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E58" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="F58" s="7"/>
     </row>
@@ -1970,13 +1972,13 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="E59" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="F59" s="12"/>
     </row>
@@ -1985,16 +1987,16 @@
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="25.5">
@@ -2002,16 +2004,16 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D61" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E61" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="38.25">
@@ -2019,16 +2021,16 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>122</v>
+        <v>162</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="76.5">
@@ -2036,13 +2038,13 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="25.5">
@@ -2050,16 +2052,16 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C64" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D64" s="1" t="s">
-        <v>126</v>
-      </c>
       <c r="E64" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="38.25">
@@ -2067,16 +2069,16 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>128</v>
+        <v>163</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="38.25">
@@ -2084,13 +2086,13 @@
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="25.5">
@@ -2098,13 +2100,13 @@
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="25.5">
@@ -2112,13 +2114,13 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C68" s="1" t="s">
-        <v>136</v>
-      </c>
       <c r="E68" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="51">
@@ -2126,13 +2128,13 @@
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="89.25">
@@ -2140,13 +2142,13 @@
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="25.5">
@@ -2154,13 +2156,13 @@
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="38.25">
@@ -2168,13 +2170,13 @@
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="25.5">
@@ -2182,13 +2184,13 @@
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="114.75">
@@ -2196,13 +2198,13 @@
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F74" s="12"/>
     </row>
@@ -2211,10 +2213,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C75" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="51">
@@ -2222,13 +2224,13 @@
         <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="51">
@@ -2236,13 +2238,13 @@
         <v>76</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="38.25">
@@ -2250,13 +2252,13 @@
         <v>77</v>
       </c>
       <c r="B78" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="25.5">
@@ -2264,13 +2266,13 @@
         <v>78</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C79" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D79" s="13" t="s">
         <v>155</v>
-      </c>
-      <c r="D79" s="13" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="38.25">
@@ -2278,13 +2280,13 @@
         <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="38.25">
@@ -2292,13 +2294,13 @@
         <v>80</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="25.5">
@@ -2306,13 +2308,13 @@
         <v>81</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>44</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="25.5">
@@ -2320,13 +2322,24 @@
         <v>82</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="30">
+      <c r="A84" s="1">
+        <v>83</v>
+      </c>
+      <c r="B84" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="C84" s="11" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -2354,10 +2367,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCellId="1" sqref="A84:E84 A1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -2370,10 +2385,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCellId="1" sqref="A84:E84 A1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>

</xml_diff>